<commit_message>
EPBDS small test modification.
</commit_message>
<xml_diff>
--- a/WSFrontend/trunk/org.openl.rules.ruleservice/test-resources/multi-module_overloaded/project3/Module3_1.xlsx
+++ b/WSFrontend/trunk/org.openl.rules.ruleservice/test-resources/multi-module_overloaded/project3/Module3_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>properties</t>
   </si>
@@ -34,7 +34,34 @@
     <t>lob3_1</t>
   </si>
   <si>
-    <t>return "Hello3" ;</t>
+    <t>return hello3() ;</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>dependency</t>
+  </si>
+  <si>
+    <t>Module3_2</t>
+  </si>
+  <si>
+    <t>From dependency</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>Rules String hello3()</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>String res</t>
+  </si>
+  <si>
+    <t>=return helloFromDependency() ;</t>
   </si>
 </sst>
 </file>
@@ -59,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -82,15 +109,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -441,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E5"/>
+  <dimension ref="B3:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,10 +560,73 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="9">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>